<commit_message>
Easier to change values
</commit_message>
<xml_diff>
--- a/csgo_prices.xlsx
+++ b/csgo_prices.xlsx
@@ -496,13 +496,13 @@
         <v>28.1</v>
       </c>
       <c r="C2" s="1">
-        <v>22.63</v>
+        <v>23.49</v>
       </c>
       <c r="D2" s="1">
-        <v>-5.470000000000002</v>
+        <v>-4.610000000000003</v>
       </c>
       <c r="E2" s="2">
-        <v>-0.1946619217081851</v>
+        <v>-0.1640569395017795</v>
       </c>
       <c r="G2" s="4">
         <f>SUM(B2:B6)</f>
@@ -525,13 +525,13 @@
         <v>7.66</v>
       </c>
       <c r="C3" s="1">
-        <v>14.92</v>
+        <v>15.02</v>
       </c>
       <c r="D3" s="1">
-        <v>7.26</v>
+        <v>7.359999999999999</v>
       </c>
       <c r="E3" s="2">
-        <v>0.9477806788511749</v>
+        <v>0.9608355091383811</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -542,13 +542,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>11.81</v>
+        <v>13.43</v>
       </c>
       <c r="D4" s="1">
-        <v>-1.19</v>
+        <v>0.4299999999999997</v>
       </c>
       <c r="E4" s="2">
-        <v>-0.0915384615384615</v>
+        <v>0.03307692307692305</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -559,13 +559,13 @@
         <v>11.16</v>
       </c>
       <c r="C5" s="1">
-        <v>10.77</v>
+        <v>11.5</v>
       </c>
       <c r="D5" s="1">
-        <v>-0.3900000000000006</v>
+        <v>0.3399999999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>-0.03494623655913984</v>
+        <v>0.03046594982078852</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -576,13 +576,13 @@
         <v>3.26</v>
       </c>
       <c r="C6" s="1">
-        <v>4.86</v>
+        <v>4.65</v>
       </c>
       <c r="D6" s="1">
-        <v>1.600000000000001</v>
+        <v>1.390000000000001</v>
       </c>
       <c r="E6" s="2">
-        <v>0.4907975460122702</v>
+        <v>0.4263803680981597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>